<commit_message>
update cage role and permission file, fix role name
</commit_message>
<xml_diff>
--- a/role_permission_files/Cage_RoleAndPermission_v0.13.xlsx
+++ b/role_permission_files/Cage_RoleAndPermission_v0.13.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="153">
   <si>
     <t>Version</t>
   </si>
@@ -497,6 +497,21 @@
   </si>
   <si>
     <t>search_audit_log</t>
+  </si>
+  <si>
+    <t>cashier</t>
+  </si>
+  <si>
+    <t>cage_manager</t>
+  </si>
+  <si>
+    <t>shift_manager</t>
+  </si>
+  <si>
+    <t>marketing_counter</t>
+  </si>
+  <si>
+    <t>it_specialist</t>
   </si>
 </sst>
 </file>
@@ -1038,9 +1053,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1050,18 +1077,45 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1069,45 +1123,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1405,12 +1420,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
     </row>
     <row r="3" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C3" s="3" t="s">
@@ -1867,38 +1882,38 @@
       </c>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="79" t="s">
+      <c r="B3" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="79" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="79" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="79" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="79" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="80"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="58" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="58" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="58" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="58" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="59"/>
     </row>
     <row r="4" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="62" t="s">
         <v>37</v>
       </c>
       <c r="B4" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="71" t="s">
+      <c r="C4" s="65" t="s">
         <v>40</v>
       </c>
       <c r="D4" s="53" t="s">
@@ -1919,11 +1934,11 @@
       <c r="I4" s="53"/>
     </row>
     <row r="5" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="58"/>
+      <c r="A5" s="62"/>
       <c r="B5" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="72"/>
+      <c r="C5" s="66"/>
       <c r="D5" s="53" t="s">
         <v>11</v>
       </c>
@@ -1942,11 +1957,11 @@
       <c r="I5" s="53"/>
     </row>
     <row r="6" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="58"/>
+      <c r="A6" s="62"/>
       <c r="B6" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="72"/>
+      <c r="C6" s="66"/>
       <c r="D6" s="53" t="s">
         <v>11</v>
       </c>
@@ -1965,11 +1980,11 @@
       <c r="I6" s="53"/>
     </row>
     <row r="7" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="58"/>
+      <c r="A7" s="62"/>
       <c r="B7" s="53" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="72"/>
+      <c r="C7" s="66"/>
       <c r="D7" s="53" t="s">
         <v>11</v>
       </c>
@@ -1988,13 +2003,13 @@
       <c r="I7" s="53"/>
     </row>
     <row r="8" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="60" t="s">
+      <c r="A8" s="64" t="s">
         <v>38</v>
       </c>
       <c r="B8" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="73"/>
+      <c r="C8" s="67"/>
       <c r="D8" s="53" t="s">
         <v>11</v>
       </c>
@@ -2013,11 +2028,11 @@
       <c r="I8" s="53"/>
     </row>
     <row r="9" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="60"/>
+      <c r="A9" s="64"/>
       <c r="B9" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="74" t="s">
+      <c r="C9" s="68" t="s">
         <v>41</v>
       </c>
       <c r="D9" s="44" t="s">
@@ -2036,11 +2051,11 @@
       <c r="I9" s="46"/>
     </row>
     <row r="10" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="60"/>
+      <c r="A10" s="64"/>
       <c r="B10" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="75"/>
+      <c r="C10" s="69"/>
       <c r="D10" s="44" t="s">
         <v>11</v>
       </c>
@@ -2057,11 +2072,11 @@
       <c r="I10" s="46"/>
     </row>
     <row r="11" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="60"/>
+      <c r="A11" s="64"/>
       <c r="B11" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="75"/>
+      <c r="C11" s="69"/>
       <c r="D11" s="44" t="s">
         <v>11</v>
       </c>
@@ -2072,11 +2087,11 @@
       <c r="I11" s="46"/>
     </row>
     <row r="12" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="60"/>
+      <c r="A12" s="64"/>
       <c r="B12" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="75"/>
+      <c r="C12" s="69"/>
       <c r="D12" s="44" t="s">
         <v>11</v>
       </c>
@@ -2093,11 +2108,11 @@
       <c r="I12" s="46"/>
     </row>
     <row r="13" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="60"/>
+      <c r="A13" s="64"/>
       <c r="B13" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="75"/>
+      <c r="C13" s="69"/>
       <c r="D13" s="44" t="s">
         <v>11</v>
       </c>
@@ -2112,11 +2127,11 @@
       <c r="I13" s="46"/>
     </row>
     <row r="14" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="60"/>
+      <c r="A14" s="64"/>
       <c r="B14" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="75"/>
+      <c r="C14" s="69"/>
       <c r="D14" s="44" t="s">
         <v>11</v>
       </c>
@@ -2133,11 +2148,11 @@
       <c r="I14" s="46"/>
     </row>
     <row r="15" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="60"/>
+      <c r="A15" s="64"/>
       <c r="B15" s="52" t="s">
         <v>131</v>
       </c>
-      <c r="C15" s="75"/>
+      <c r="C15" s="69"/>
       <c r="D15" s="52" t="s">
         <v>11</v>
       </c>
@@ -2148,11 +2163,11 @@
       <c r="I15" s="46"/>
     </row>
     <row r="16" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="60"/>
+      <c r="A16" s="64"/>
       <c r="B16" s="52" t="s">
         <v>132</v>
       </c>
-      <c r="C16" s="75"/>
+      <c r="C16" s="69"/>
       <c r="D16" s="52" t="s">
         <v>11</v>
       </c>
@@ -2163,11 +2178,11 @@
       <c r="I16" s="46"/>
     </row>
     <row r="17" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="60"/>
+      <c r="A17" s="64"/>
       <c r="B17" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="C17" s="76"/>
+      <c r="C17" s="70"/>
       <c r="D17" s="44" t="s">
         <v>11</v>
       </c>
@@ -2182,11 +2197,11 @@
       <c r="I17" s="46"/>
     </row>
     <row r="18" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="59" t="s">
+      <c r="A18" s="63" t="s">
         <v>39</v>
       </c>
       <c r="B18" s="42"/>
-      <c r="C18" s="59" t="s">
+      <c r="C18" s="63" t="s">
         <v>48</v>
       </c>
       <c r="D18" s="42" t="s">
@@ -2201,11 +2216,11 @@
       <c r="I18" s="43"/>
     </row>
     <row r="19" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="59"/>
+      <c r="A19" s="63"/>
       <c r="B19" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="59"/>
+      <c r="C19" s="63"/>
       <c r="D19" s="42" t="s">
         <v>11</v>
       </c>
@@ -2220,11 +2235,11 @@
       <c r="I19" s="43"/>
     </row>
     <row r="20" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="59"/>
+      <c r="A20" s="63"/>
       <c r="B20" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="59"/>
+      <c r="C20" s="63"/>
       <c r="D20" s="43" t="s">
         <v>11</v>
       </c>
@@ -2258,127 +2273,127 @@
       <c r="I21" s="47"/>
     </row>
     <row r="22" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="77" t="s">
+      <c r="A22" s="61" t="s">
         <v>82</v>
       </c>
-      <c r="B22" s="78" t="s">
+      <c r="B22" s="57" t="s">
         <v>84</v>
       </c>
-      <c r="C22" s="77" t="s">
+      <c r="C22" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="D22" s="78" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="78"/>
-      <c r="F22" s="78"/>
-      <c r="G22" s="78"/>
-      <c r="H22" s="78"/>
-      <c r="I22" s="78" t="s">
+      <c r="D22" s="57" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="57"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="57"/>
+      <c r="I22" s="57" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="77"/>
-      <c r="B23" s="78" t="s">
+      <c r="A23" s="61"/>
+      <c r="B23" s="57" t="s">
         <v>83</v>
       </c>
-      <c r="C23" s="77"/>
-      <c r="D23" s="78" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" s="78"/>
-      <c r="F23" s="78"/>
-      <c r="G23" s="78"/>
-      <c r="H23" s="78"/>
-      <c r="I23" s="78" t="s">
+      <c r="C23" s="61"/>
+      <c r="D23" s="57" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="57"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="57"/>
+      <c r="H23" s="57"/>
+      <c r="I23" s="57" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="77"/>
-      <c r="B24" s="78" t="s">
+      <c r="A24" s="61"/>
+      <c r="B24" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="C24" s="77"/>
-      <c r="D24" s="78" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="78"/>
-      <c r="F24" s="78"/>
-      <c r="G24" s="78"/>
-      <c r="H24" s="78"/>
-      <c r="I24" s="78" t="s">
+      <c r="C24" s="61"/>
+      <c r="D24" s="57" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="57"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="57" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="77"/>
-      <c r="B25" s="78" t="s">
+      <c r="A25" s="61"/>
+      <c r="B25" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="C25" s="77" t="s">
+      <c r="C25" s="61" t="s">
         <v>90</v>
       </c>
-      <c r="D25" s="78" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" s="78"/>
-      <c r="F25" s="78"/>
-      <c r="G25" s="78"/>
-      <c r="H25" s="78"/>
-      <c r="I25" s="78" t="s">
+      <c r="D25" s="57" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="57"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="57"/>
+      <c r="H25" s="57"/>
+      <c r="I25" s="57" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="77"/>
-      <c r="B26" s="78" t="s">
+      <c r="A26" s="61"/>
+      <c r="B26" s="57" t="s">
         <v>87</v>
       </c>
-      <c r="C26" s="77"/>
-      <c r="D26" s="78" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" s="78"/>
-      <c r="F26" s="78"/>
-      <c r="G26" s="78"/>
-      <c r="H26" s="78"/>
-      <c r="I26" s="78" t="s">
+      <c r="C26" s="61"/>
+      <c r="D26" s="57" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="57" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="77"/>
-      <c r="B27" s="78" t="s">
+      <c r="A27" s="61"/>
+      <c r="B27" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="C27" s="77"/>
-      <c r="D27" s="78" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27" s="78"/>
-      <c r="F27" s="78"/>
-      <c r="G27" s="78"/>
-      <c r="H27" s="78"/>
-      <c r="I27" s="78" t="s">
+      <c r="C27" s="61"/>
+      <c r="D27" s="57" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="57"/>
+      <c r="F27" s="57"/>
+      <c r="G27" s="57"/>
+      <c r="H27" s="57"/>
+      <c r="I27" s="57" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="77"/>
-      <c r="B28" s="78" t="s">
+      <c r="A28" s="61"/>
+      <c r="B28" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="C28" s="77"/>
-      <c r="D28" s="78" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" s="78"/>
-      <c r="F28" s="78"/>
-      <c r="G28" s="78"/>
-      <c r="H28" s="78"/>
-      <c r="I28" s="78" t="s">
+      <c r="C28" s="61"/>
+      <c r="D28" s="57" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="57"/>
+      <c r="F28" s="57"/>
+      <c r="G28" s="57"/>
+      <c r="H28" s="57"/>
+      <c r="I28" s="57" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2485,7 +2500,7 @@
   <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2508,19 +2523,19 @@
         <v>119</v>
       </c>
       <c r="C1" s="41" t="s">
-        <v>50</v>
+        <v>148</v>
       </c>
       <c r="D1" s="41" t="s">
-        <v>53</v>
+        <v>149</v>
       </c>
       <c r="E1" s="41" t="s">
-        <v>51</v>
+        <v>150</v>
       </c>
       <c r="F1" s="41" t="s">
-        <v>52</v>
+        <v>151</v>
       </c>
       <c r="G1" s="41" t="s">
-        <v>93</v>
+        <v>152</v>
       </c>
       <c r="H1" s="56" t="s">
         <v>120</v>
@@ -3299,10 +3314,10 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="78" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="66"/>
+      <c r="B2" s="79"/>
       <c r="C2" s="28" t="s">
         <v>9</v>
       </c>
@@ -3329,16 +3344,16 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="72" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="63" t="s">
+      <c r="D3" s="77" t="s">
         <v>18</v>
       </c>
       <c r="E3" s="34" t="s">
@@ -3355,12 +3370,12 @@
       <c r="L3" s="38"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="62"/>
-      <c r="B4" s="62"/>
+      <c r="A4" s="76"/>
+      <c r="B4" s="76"/>
       <c r="C4" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="64"/>
+      <c r="D4" s="75"/>
       <c r="E4" s="30" t="s">
         <v>11</v>
       </c>
@@ -3375,12 +3390,12 @@
       <c r="L4" s="30"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="62"/>
-      <c r="B5" s="62"/>
+      <c r="A5" s="76"/>
+      <c r="B5" s="76"/>
       <c r="C5" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="64"/>
+      <c r="D5" s="75"/>
       <c r="E5" s="30" t="s">
         <v>11</v>
       </c>
@@ -3395,12 +3410,12 @@
       <c r="L5" s="30"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="62"/>
-      <c r="B6" s="62"/>
+      <c r="A6" s="76"/>
+      <c r="B6" s="76"/>
       <c r="C6" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="64"/>
+      <c r="D6" s="75"/>
       <c r="E6" s="30" t="s">
         <v>11</v>
       </c>
@@ -3415,12 +3430,12 @@
       <c r="L6" s="30"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="62"/>
-      <c r="B7" s="62"/>
+      <c r="A7" s="76"/>
+      <c r="B7" s="76"/>
       <c r="C7" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="64"/>
+      <c r="D7" s="75"/>
       <c r="E7" s="30" t="s">
         <v>11</v>
       </c>
@@ -3433,12 +3448,12 @@
       <c r="L7" s="30"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="62"/>
-      <c r="B8" s="62"/>
+      <c r="A8" s="76"/>
+      <c r="B8" s="76"/>
       <c r="C8" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="64"/>
+      <c r="D8" s="75"/>
       <c r="E8" s="30" t="s">
         <v>11</v>
       </c>
@@ -3489,10 +3504,10 @@
       <c r="A13" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="67" t="s">
+      <c r="B13" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="67"/>
+      <c r="C13" s="80"/>
       <c r="D13" s="17" t="s">
         <v>9</v>
       </c>
@@ -3520,16 +3535,16 @@
       <c r="A14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="68" t="s">
+      <c r="B14" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="68" t="s">
+      <c r="C14" s="71" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="69" t="s">
+      <c r="E14" s="73" t="s">
         <v>18</v>
       </c>
       <c r="F14" s="33" t="s">
@@ -3548,15 +3563,15 @@
       <c r="M14" s="26"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="64" t="s">
+      <c r="A15" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="68"/>
-      <c r="C15" s="68"/>
+      <c r="B15" s="71"/>
+      <c r="C15" s="71"/>
       <c r="D15" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="69"/>
+      <c r="E15" s="73"/>
       <c r="F15" s="15" t="s">
         <v>11</v>
       </c>
@@ -3573,13 +3588,13 @@
       <c r="M15" s="18"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="64"/>
-      <c r="B16" s="68"/>
-      <c r="C16" s="68"/>
+      <c r="A16" s="75"/>
+      <c r="B16" s="71"/>
+      <c r="C16" s="71"/>
       <c r="D16" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="69"/>
+      <c r="E16" s="73"/>
       <c r="F16" s="15" t="s">
         <v>11</v>
       </c>
@@ -3596,13 +3611,13 @@
       <c r="M16" s="18"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="64"/>
-      <c r="B17" s="68"/>
-      <c r="C17" s="68"/>
+      <c r="A17" s="75"/>
+      <c r="B17" s="71"/>
+      <c r="C17" s="71"/>
       <c r="D17" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="69"/>
+      <c r="E17" s="73"/>
       <c r="F17" s="15" t="s">
         <v>11</v>
       </c>
@@ -3619,13 +3634,13 @@
       <c r="M17" s="18"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="64"/>
-      <c r="B18" s="68"/>
-      <c r="C18" s="68"/>
+      <c r="A18" s="75"/>
+      <c r="B18" s="71"/>
+      <c r="C18" s="71"/>
       <c r="D18" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="69"/>
+      <c r="E18" s="73"/>
       <c r="F18" s="15" t="s">
         <v>11</v>
       </c>
@@ -3640,13 +3655,13 @@
       <c r="M18" s="18"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="64"/>
-      <c r="B19" s="68"/>
-      <c r="C19" s="68"/>
+      <c r="A19" s="75"/>
+      <c r="B19" s="71"/>
+      <c r="C19" s="71"/>
       <c r="D19" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="69"/>
+      <c r="E19" s="73"/>
       <c r="F19" s="15" t="s">
         <v>11</v>
       </c>
@@ -3661,15 +3676,15 @@
       <c r="M19" s="18"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="64" t="s">
+      <c r="A20" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="68"/>
-      <c r="C20" s="68"/>
+      <c r="B20" s="71"/>
+      <c r="C20" s="71"/>
       <c r="D20" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="69"/>
+      <c r="E20" s="73"/>
       <c r="F20" s="15" t="s">
         <v>11</v>
       </c>
@@ -3684,13 +3699,13 @@
       <c r="M20" s="25"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="64"/>
-      <c r="B21" s="68"/>
-      <c r="C21" s="68"/>
+      <c r="A21" s="75"/>
+      <c r="B21" s="71"/>
+      <c r="C21" s="71"/>
       <c r="D21" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="69"/>
+      <c r="E21" s="73"/>
       <c r="F21" s="15" t="s">
         <v>11</v>
       </c>
@@ -3705,13 +3720,13 @@
       <c r="M21" s="25"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="64"/>
-      <c r="B22" s="68"/>
-      <c r="C22" s="68"/>
+      <c r="A22" s="75"/>
+      <c r="B22" s="71"/>
+      <c r="C22" s="71"/>
       <c r="D22" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="69"/>
+      <c r="E22" s="73"/>
       <c r="F22" s="15" t="s">
         <v>11</v>
       </c>
@@ -3726,13 +3741,13 @@
       <c r="M22" s="25"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="64"/>
-      <c r="B23" s="68"/>
-      <c r="C23" s="68"/>
+      <c r="A23" s="75"/>
+      <c r="B23" s="71"/>
+      <c r="C23" s="71"/>
       <c r="D23" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E23" s="69"/>
+      <c r="E23" s="73"/>
       <c r="F23" s="15" t="s">
         <v>11</v>
       </c>
@@ -3747,13 +3762,13 @@
       <c r="M23" s="25"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="64"/>
-      <c r="B24" s="68"/>
-      <c r="C24" s="68"/>
+      <c r="A24" s="75"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="71"/>
       <c r="D24" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="69"/>
+      <c r="E24" s="73"/>
       <c r="F24" s="15" t="s">
         <v>11</v>
       </c>
@@ -3768,15 +3783,15 @@
       <c r="M24" s="25"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="64" t="s">
+      <c r="A25" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="68"/>
-      <c r="C25" s="68"/>
+      <c r="B25" s="71"/>
+      <c r="C25" s="71"/>
       <c r="D25" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="69"/>
+      <c r="E25" s="73"/>
       <c r="F25" s="15" t="s">
         <v>11</v>
       </c>
@@ -3791,13 +3806,13 @@
       <c r="M25" s="25"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="64"/>
-      <c r="B26" s="68"/>
-      <c r="C26" s="68"/>
+      <c r="A26" s="75"/>
+      <c r="B26" s="71"/>
+      <c r="C26" s="71"/>
       <c r="D26" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E26" s="69"/>
+      <c r="E26" s="73"/>
       <c r="F26" s="15" t="s">
         <v>11</v>
       </c>
@@ -3812,13 +3827,13 @@
       <c r="M26" s="25"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="64"/>
-      <c r="B27" s="68"/>
-      <c r="C27" s="68"/>
+      <c r="A27" s="75"/>
+      <c r="B27" s="71"/>
+      <c r="C27" s="71"/>
       <c r="D27" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E27" s="69"/>
+      <c r="E27" s="73"/>
       <c r="F27" s="15" t="s">
         <v>11</v>
       </c>
@@ -3833,13 +3848,13 @@
       <c r="M27" s="25"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="64"/>
-      <c r="B28" s="68"/>
-      <c r="C28" s="68"/>
+      <c r="A28" s="75"/>
+      <c r="B28" s="71"/>
+      <c r="C28" s="71"/>
       <c r="D28" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E28" s="69"/>
+      <c r="E28" s="73"/>
       <c r="F28" s="15" t="s">
         <v>11</v>
       </c>
@@ -3854,13 +3869,13 @@
       <c r="M28" s="25"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="64"/>
-      <c r="B29" s="61"/>
-      <c r="C29" s="61"/>
+      <c r="A29" s="75"/>
+      <c r="B29" s="72"/>
+      <c r="C29" s="72"/>
       <c r="D29" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="70"/>
+      <c r="E29" s="74"/>
       <c r="F29" s="15" t="s">
         <v>11</v>
       </c>
@@ -3903,17 +3918,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B3:B8"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="D3:D8"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:B29"/>
     <mergeCell ref="C14:C29"/>
     <mergeCell ref="E14:E29"/>
     <mergeCell ref="A15:A19"/>
     <mergeCell ref="A20:A24"/>
     <mergeCell ref="A25:A29"/>
-    <mergeCell ref="B3:B8"/>
-    <mergeCell ref="A3:A8"/>
-    <mergeCell ref="D3:D8"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>